<commit_message>
Cahier des charges - conclusion
Cahier des charges - conclusion
Mise à jour du planning

Temps travail : 0.5 heures
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC16CC8-658E-41F2-8D9A-0EC3A7224249}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5ACF4D-16C6-47C8-A923-515623DF7696}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="1" r:id="rId1"/>
     <sheet name="SPRINTS" sheetId="2" r:id="rId2"/>
+    <sheet name="SPRINT 0" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>DÉPÔT TB</t>
   </si>
@@ -109,6 +110,27 @@
   </si>
   <si>
     <t>Dégrossir l'information, créer le cahier des charges</t>
+  </si>
+  <si>
+    <t>Rencontre professeur, discussions des objectifs du travail</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Quoi</t>
+  </si>
+  <si>
+    <t>Temps (h)</t>
+  </si>
+  <si>
+    <t>Introduction du cahier des charges</t>
+  </si>
+  <si>
+    <t>Mise en page cahier des charges</t>
+  </si>
+  <si>
+    <t>Conclusion du cahier des charges</t>
   </si>
 </sst>
 </file>
@@ -168,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -182,6 +204,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,7 +525,7 @@
   <dimension ref="A3:G52"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -541,7 +564,9 @@
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="5"/>
       <c r="E4" s="3"/>
@@ -580,9 +605,6 @@
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1521,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8302CA45-31B6-4463-AEAD-E85456601763}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1547,7 +1569,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="6">
-        <v>43886</v>
+        <v>43879</v>
       </c>
       <c r="C2" s="6">
         <v>43899</v>
@@ -1615,6 +1637,79 @@
         <v>44041</v>
       </c>
       <c r="D7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C400973-BE12-4374-A59C-9A57E0EEF3E6}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="7">
+        <v>43879</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B4" s="7">
+        <v>43885</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="7">
+        <v>43885</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="7">
+        <v>43885</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cahier des charges - problématiques - sécurité
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5ACF4D-16C6-47C8-A923-515623DF7696}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22751FFB-D0FD-459C-836A-EA08612BE998}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>DÉPÔT TB</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Conclusion du cahier des charges</t>
+  </si>
+  <si>
+    <t>Problématique du cahier des charges</t>
   </si>
 </sst>
 </file>
@@ -1645,10 +1648,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C400973-BE12-4374-A59C-9A57E0EEF3E6}">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1711,6 +1714,17 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="7">
+        <v>43885</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cahier des charges - problématiques - interface web
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22751FFB-D0FD-459C-836A-EA08612BE998}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A411C7E1-EDE4-41B8-A494-AC31A253C935}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
@@ -1648,10 +1648,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C400973-BE12-4374-A59C-9A57E0EEF3E6}">
-  <dimension ref="B2:D7"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1722,8 +1722,11 @@
         <v>30</v>
       </c>
       <c r="D7">
-        <v>2</v>
-      </c>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cahier des charges - Travail à effectuer
Cahier des charges - Travail à effectuer
Mise à jour planification
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A411C7E1-EDE4-41B8-A494-AC31A253C935}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2A959E-D26C-41FB-85D2-5BF1DD43CA58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>DÉPÔT TB</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Problématique du cahier des charges</t>
+  </si>
+  <si>
+    <t>Travail à éffectuer du cahier des charges</t>
   </si>
 </sst>
 </file>
@@ -1651,7 +1654,7 @@
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1726,7 +1729,15 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B8" s="7"/>
+      <c r="B8" s="7">
+        <v>43885</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cahier des charges - planif + travail a effectuer
Cahier des charges - planif + travail a effectuer
Modification de l'échéancier dans le planning (durée des sprints)
Ajout d'information dans le planning
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2A959E-D26C-41FB-85D2-5BF1DD43CA58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12850629-0FBA-45B5-B92B-AD03D7E6FA2E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
@@ -33,38 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>DÉPÔT TB</t>
-  </si>
-  <si>
-    <t>rencontre prof. 16h
-DEBUT SPRINT 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
   <si>
-    <t>rencontre prof. 16h
-DEBUT SPRINT 3</t>
-  </si>
-  <si>
     <t>FIN SPRINT 2</t>
   </si>
   <si>
-    <t>rencontre prof. 16h
-DEBUT SPRINT 4</t>
-  </si>
-  <si>
     <t>FIN SPRINT 3</t>
-  </si>
-  <si>
-    <t>rencontre prof. 16h
-DEBUT SPRINT 5</t>
-  </si>
-  <si>
-    <t>rencontre prof. 16h
-FIN TB, RENDU</t>
   </si>
   <si>
     <t>FIN SPRINT 5</t>
@@ -137,6 +114,60 @@
   </si>
   <si>
     <t>Travail à éffectuer du cahier des charges</t>
+  </si>
+  <si>
+    <t>Planification du cahier des charges</t>
+  </si>
+  <si>
+    <t>DEBUT SPRINT 2</t>
+  </si>
+  <si>
+    <t>DEBUT SPRINT 3</t>
+  </si>
+  <si>
+    <t>DEBUT SPRINT 4</t>
+  </si>
+  <si>
+    <t>FIN SPRINT 4</t>
+  </si>
+  <si>
+    <t>DEBUT SPRINT 5</t>
+  </si>
+  <si>
+    <t>DEBUT SPRINT 6</t>
+  </si>
+  <si>
+    <t>FIN SPRINT 6</t>
+  </si>
+  <si>
+    <t>DEBUT SPRINT 7</t>
+  </si>
+  <si>
+    <t>FIN SPRINT 8</t>
+  </si>
+  <si>
+    <t>DEBUT SPRINT 9</t>
+  </si>
+  <si>
+    <t>FIN SPRINT 9</t>
+  </si>
+  <si>
+    <t>DEBUT SPRINT 10</t>
+  </si>
+  <si>
+    <t>FIN SPRINT 10</t>
+  </si>
+  <si>
+    <t>DEBUT SPRINT 11</t>
+  </si>
+  <si>
+    <t>FIN SPRINT 11</t>
+  </si>
+  <si>
+    <t>Rendu TB</t>
+  </si>
+  <si>
+    <t>Echéancier du cahier des charges</t>
   </si>
 </sst>
 </file>
@@ -530,8 +561,8 @@
   </sheetPr>
   <dimension ref="A3:G52"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -571,7 +602,7 @@
     <row r="4" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="5"/>
@@ -655,7 +686,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -690,7 +721,7 @@
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="5"/>
@@ -771,8 +802,12 @@
     <row r="14" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -849,8 +884,12 @@
     <row r="18" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -888,12 +927,8 @@
     <row r="20" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -931,8 +966,12 @@
     <row r="22" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1009,8 +1048,12 @@
     <row r="26" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1048,12 +1091,8 @@
     <row r="28" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1091,8 +1130,12 @@
     <row r="30" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1169,8 +1212,12 @@
     <row r="34" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -1208,12 +1255,8 @@
     <row r="36" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -1251,8 +1294,12 @@
     <row r="38" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -1329,8 +1376,12 @@
     <row r="42" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="C42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -1369,9 +1420,7 @@
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="D44" s="5"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -1409,8 +1458,12 @@
     <row r="46" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -1486,13 +1539,13 @@
     </row>
     <row r="50" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="3"/>
-      <c r="B50" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="B50" s="3"/>
       <c r="C50" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -1532,9 +1585,7 @@
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
@@ -1550,7 +1601,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1561,18 +1612,18 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6">
         <v>43879</v>
@@ -1581,12 +1632,12 @@
         <v>43899</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6">
         <v>43909</v>
@@ -1598,7 +1649,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6">
         <v>43937</v>
@@ -1610,7 +1661,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6">
         <v>43965</v>
@@ -1622,7 +1673,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6" s="6">
         <v>43993</v>
@@ -1634,7 +1685,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="6">
         <v>44021</v>
@@ -1651,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C400973-BE12-4374-A59C-9A57E0EEF3E6}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1664,13 +1715,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
@@ -1678,7 +1729,7 @@
         <v>43879</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1689,7 +1740,7 @@
         <v>43885</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1700,7 +1751,7 @@
         <v>43885</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -1711,7 +1762,7 @@
         <v>43885</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>0.5</v>
@@ -1722,7 +1773,7 @@
         <v>43885</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>2.5</v>
@@ -1733,10 +1784,38 @@
         <v>43885</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="7">
+        <v>43889</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="7">
+        <v>43889</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D12">
+        <f>SUM(D3:D10)</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour planification
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12850629-0FBA-45B5-B92B-AD03D7E6FA2E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10475DA-5755-4C0E-947E-E6CEA23ED4D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Echéancier du cahier des charges</t>
+  </si>
+  <si>
+    <t>Rendus du cahier des charges</t>
+  </si>
+  <si>
+    <t>Mise en page et relecture cahier des charges</t>
   </si>
 </sst>
 </file>
@@ -1702,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C400973-BE12-4374-A59C-9A57E0EEF3E6}">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1812,10 +1818,32 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B11" s="7">
+        <v>43897</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+    </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="7">
+        <v>43897</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
       <c r="D12">
-        <f>SUM(D3:D10)</f>
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D14">
+        <f>SUM(D3:D12)</f>
+        <v>9.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour planification + mise en page cahier des charges
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10475DA-5755-4C0E-947E-E6CEA23ED4D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EBC2B6-9292-49B4-B17A-9A7872CC5403}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>Mise en page et relecture cahier des charges</t>
+  </si>
+  <si>
+    <t>Rencontre TB, fin Sprint 0</t>
+  </si>
+  <si>
+    <t>Sprint 0 review, notes de séance en document annexe</t>
   </si>
 </sst>
 </file>
@@ -1708,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C400973-BE12-4374-A59C-9A57E0EEF3E6}">
-  <dimension ref="B2:D14"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1840,13 +1846,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D14">
-        <f>SUM(D3:D12)</f>
-        <v>9.5</v>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="7">
+        <v>43899</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D15">
+        <f>SUM(D3:D13)</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sprint 1 - planning + intro synthèse état de l'art
Mise en page planning sprint 1
intro synthèse de l'art + GNI
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282185A6-6D01-4428-85F9-B5C149EE52C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A5C5B-F2A8-4C44-B649-7D381D13A404}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="1" r:id="rId1"/>
     <sheet name="SPRINTS" sheetId="2" r:id="rId2"/>
     <sheet name="SPRINT 0" sheetId="3" r:id="rId3"/>
+    <sheet name="SPRINT 1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -183,6 +184,30 @@
   </si>
   <si>
     <t>Documentation sprint review 0</t>
+  </si>
+  <si>
+    <t>Lecture TOJC</t>
+  </si>
+  <si>
+    <t>Lecture rapport analyse 2020 WP1</t>
+  </si>
+  <si>
+    <t>Synthèse état de l'art - introduction</t>
+  </si>
+  <si>
+    <t>Synthèse état de l'art - GNI + Trust Project</t>
+  </si>
+  <si>
+    <t>Synthèse état de l'art - JTI + Transparency Journalism + NewsGuard</t>
+  </si>
+  <si>
+    <t>Synthèse état de l'art - comparaison</t>
+  </si>
+  <si>
+    <t>Synthèse état de l'art - conclusion</t>
+  </si>
+  <si>
+    <t>Sprint 1 review, notes de séance en document annexe</t>
   </si>
 </sst>
 </file>
@@ -1719,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C400973-BE12-4374-A59C-9A57E0EEF3E6}">
   <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1886,4 +1911,136 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A059C0DF-3E9D-4D01-B549-9733ADE07856}">
+  <dimension ref="B2:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="7">
+        <v>43904</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B4" s="7">
+        <v>43904</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="7">
+        <v>43911</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="7">
+        <v>43911</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="7">
+        <v>43911</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="7">
+        <v>43911</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="7">
+        <v>43911</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D16">
+        <f>SUM(D3:D9)</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sprint 1 - Rendu Etat de l'Art I
Etat de l'art conclusion + tableau résumé + modification planning
Mise à jour final état de l'art I
Mise en page
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A5C5B-F2A8-4C44-B649-7D381D13A404}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD44112-BB36-4615-B818-322C402B52E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -204,10 +204,16 @@
     <t>Synthèse état de l'art - comparaison</t>
   </si>
   <si>
-    <t>Synthèse état de l'art - conclusion</t>
-  </si>
-  <si>
     <t>Sprint 1 review, notes de séance en document annexe</t>
+  </si>
+  <si>
+    <t>Lecture du CWA 17493 JTI</t>
+  </si>
+  <si>
+    <t>Mise en page état de l'art et conclusion</t>
+  </si>
+  <si>
+    <t>Rencontre sur Teams + Sprint review et spring 2 planning</t>
   </si>
 </sst>
 </file>
@@ -605,18 +611,18 @@
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43878</v>
       </c>
@@ -639,7 +645,7 @@
         <v>43884</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -650,7 +656,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>G3+1</f>
         <v>43885</v>
@@ -680,7 +686,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -688,7 +694,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>G5+1</f>
         <v>43892</v>
@@ -718,7 +724,7 @@
         <v>43898</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -729,7 +735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>G7+1</f>
         <v>43899</v>
@@ -759,7 +765,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -770,7 +776,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>G9+1</f>
         <v>43906</v>
@@ -800,7 +806,7 @@
         <v>43912</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -809,7 +815,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>G11+1</f>
         <v>43913</v>
@@ -839,7 +845,7 @@
         <v>43919</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -852,7 +858,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f>G13+1</f>
         <v>43920</v>
@@ -882,7 +888,7 @@
         <v>43926</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -891,7 +897,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f>G15+1</f>
         <v>43927</v>
@@ -921,7 +927,7 @@
         <v>43933</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
@@ -934,7 +940,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f>G17+1</f>
         <v>43934</v>
@@ -964,7 +970,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -973,7 +979,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f>G19+1</f>
         <v>43941</v>
@@ -1003,7 +1009,7 @@
         <v>43947</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
@@ -1016,7 +1022,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f>G21+1</f>
         <v>43948</v>
@@ -1046,7 +1052,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1055,7 +1061,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f>G23+1</f>
         <v>43955</v>
@@ -1085,7 +1091,7 @@
         <v>43961</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
@@ -1098,7 +1104,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f>G25+1</f>
         <v>43962</v>
@@ -1128,7 +1134,7 @@
         <v>43968</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1137,7 +1143,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f>G27+1</f>
         <v>43969</v>
@@ -1167,7 +1173,7 @@
         <v>43975</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
@@ -1180,7 +1186,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f>G29+1</f>
         <v>43976</v>
@@ -1210,7 +1216,7 @@
         <v>43982</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1219,7 +1225,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f>G31+1</f>
         <v>43983</v>
@@ -1249,7 +1255,7 @@
         <v>43989</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
@@ -1262,7 +1268,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f>G33+1</f>
         <v>43990</v>
@@ -1292,7 +1298,7 @@
         <v>43996</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1301,7 +1307,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f>G35+1</f>
         <v>43997</v>
@@ -1331,7 +1337,7 @@
         <v>44003</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -1344,7 +1350,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f>G37+1</f>
         <v>44004</v>
@@ -1374,7 +1380,7 @@
         <v>44010</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1383,7 +1389,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f>G39+1</f>
         <v>44011</v>
@@ -1413,7 +1419,7 @@
         <v>44017</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
@@ -1426,7 +1432,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f>G41+1</f>
         <v>44018</v>
@@ -1456,7 +1462,7 @@
         <v>44024</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1465,7 +1471,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f>G43+1</f>
         <v>44025</v>
@@ -1495,7 +1501,7 @@
         <v>44031</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
@@ -1508,7 +1514,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <f>G45+1</f>
         <v>44032</v>
@@ -1538,7 +1544,7 @@
         <v>44038</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1547,7 +1553,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f>G47+1</f>
         <v>44039</v>
@@ -1577,7 +1583,7 @@
         <v>44045</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="5" t="s">
@@ -1590,7 +1596,7 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f>G49+1</f>
         <v>44046</v>
@@ -1620,7 +1626,7 @@
         <v>44052</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="4" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1644,12 +1650,12 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="40.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>10</v>
@@ -1661,7 +1667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1687,7 +1693,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1699,7 +1705,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1711,7 +1717,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1723,7 +1729,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1748,12 +1754,12 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -1764,7 +1770,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43879</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43885</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43885</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43885</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43885</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43885</v>
       </c>
@@ -1830,7 +1836,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43889</v>
       </c>
@@ -1841,7 +1847,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>43889</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>43897</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>43897</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>43899</v>
       </c>
@@ -1885,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>43899</v>
       </c>
@@ -1896,13 +1902,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D15">
         <f>SUM(D3:D14)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>47</v>
       </c>
@@ -1915,18 +1921,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A059C0DF-3E9D-4D01-B549-9733ADE07856}">
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -1937,7 +1943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43904</v>
       </c>
@@ -1948,7 +1954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43904</v>
       </c>
@@ -1959,7 +1965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43911</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43911</v>
       </c>
@@ -1981,63 +1987,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43911</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
-        <v>43911</v>
+        <v>43916</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
-        <v>43911</v>
+        <v>43916</v>
       </c>
       <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>43916</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>43916</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>SUM(D3:D11)</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>55</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B14" s="7"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D16">
-        <f>SUM(D3:D9)</f>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C17" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Etat art II - Unicheck, copyleaks, plagiarismsearch
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD44112-BB36-4615-B818-322C402B52E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D292A975-7E53-4AFB-B7C7-4BB658F0A0F0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="4" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="1" r:id="rId1"/>
     <sheet name="SPRINTS" sheetId="2" r:id="rId2"/>
     <sheet name="SPRINT 0" sheetId="3" r:id="rId3"/>
     <sheet name="SPRINT 1" sheetId="4" r:id="rId4"/>
+    <sheet name="SPRINT 2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -214,6 +215,24 @@
   </si>
   <si>
     <t>Rencontre sur Teams + Sprint review et spring 2 planning</t>
+  </si>
+  <si>
+    <t>Edubirdie Etat art</t>
+  </si>
+  <si>
+    <t>Prepostseo Etat art</t>
+  </si>
+  <si>
+    <t>plagiarismsearch Etat art</t>
+  </si>
+  <si>
+    <t>install XAMPP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copyleaks test Etat art </t>
+  </si>
+  <si>
+    <t>Unicheck Etat art</t>
   </si>
 </sst>
 </file>
@@ -611,18 +630,18 @@
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>43878</v>
       </c>
@@ -645,7 +664,7 @@
         <v>43884</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -656,7 +675,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <f>G3+1</f>
         <v>43885</v>
@@ -686,7 +705,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -694,7 +713,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f>G5+1</f>
         <v>43892</v>
@@ -724,7 +743,7 @@
         <v>43898</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -735,7 +754,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f>G7+1</f>
         <v>43899</v>
@@ -765,7 +784,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -776,7 +795,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f>G9+1</f>
         <v>43906</v>
@@ -806,7 +825,7 @@
         <v>43912</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -815,7 +834,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f>G11+1</f>
         <v>43913</v>
@@ -845,7 +864,7 @@
         <v>43919</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -858,7 +877,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f>G13+1</f>
         <v>43920</v>
@@ -888,7 +907,7 @@
         <v>43926</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -897,7 +916,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f>G15+1</f>
         <v>43927</v>
@@ -927,7 +946,7 @@
         <v>43933</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
@@ -940,7 +959,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f>G17+1</f>
         <v>43934</v>
@@ -970,7 +989,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -979,7 +998,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f>G19+1</f>
         <v>43941</v>
@@ -1009,7 +1028,7 @@
         <v>43947</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
@@ -1022,7 +1041,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f>G21+1</f>
         <v>43948</v>
@@ -1052,7 +1071,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1061,7 +1080,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f>G23+1</f>
         <v>43955</v>
@@ -1091,7 +1110,7 @@
         <v>43961</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
@@ -1104,7 +1123,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f>G25+1</f>
         <v>43962</v>
@@ -1134,7 +1153,7 @@
         <v>43968</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1143,7 +1162,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f>G27+1</f>
         <v>43969</v>
@@ -1173,7 +1192,7 @@
         <v>43975</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
@@ -1186,7 +1205,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f>G29+1</f>
         <v>43976</v>
@@ -1216,7 +1235,7 @@
         <v>43982</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1225,7 +1244,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <f>G31+1</f>
         <v>43983</v>
@@ -1255,7 +1274,7 @@
         <v>43989</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
@@ -1268,7 +1287,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <f>G33+1</f>
         <v>43990</v>
@@ -1298,7 +1317,7 @@
         <v>43996</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1307,7 +1326,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <f>G35+1</f>
         <v>43997</v>
@@ -1337,7 +1356,7 @@
         <v>44003</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -1350,7 +1369,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <f>G37+1</f>
         <v>44004</v>
@@ -1380,7 +1399,7 @@
         <v>44010</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1389,7 +1408,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <f>G39+1</f>
         <v>44011</v>
@@ -1419,7 +1438,7 @@
         <v>44017</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
@@ -1432,7 +1451,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <f>G41+1</f>
         <v>44018</v>
@@ -1462,7 +1481,7 @@
         <v>44024</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1471,7 +1490,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <f>G43+1</f>
         <v>44025</v>
@@ -1501,7 +1520,7 @@
         <v>44031</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
@@ -1514,7 +1533,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <f>G45+1</f>
         <v>44032</v>
@@ -1544,7 +1563,7 @@
         <v>44038</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1553,7 +1572,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <f>G47+1</f>
         <v>44039</v>
@@ -1583,7 +1602,7 @@
         <v>44045</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="5" t="s">
@@ -1596,7 +1615,7 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <f>G49+1</f>
         <v>44046</v>
@@ -1626,7 +1645,7 @@
         <v>44052</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1650,12 +1669,12 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>10</v>
@@ -1667,7 +1686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1681,7 +1700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1693,7 +1712,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1705,7 +1724,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1717,7 +1736,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1729,7 +1748,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1754,12 +1773,12 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -1770,7 +1789,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" s="7">
         <v>43879</v>
       </c>
@@ -1781,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" s="7">
         <v>43885</v>
       </c>
@@ -1792,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" s="7">
         <v>43885</v>
       </c>
@@ -1803,7 +1822,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="7">
         <v>43885</v>
       </c>
@@ -1814,7 +1833,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>43885</v>
       </c>
@@ -1825,7 +1844,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B8" s="7">
         <v>43885</v>
       </c>
@@ -1836,7 +1855,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B9" s="7">
         <v>43889</v>
       </c>
@@ -1847,7 +1866,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B10" s="7">
         <v>43889</v>
       </c>
@@ -1858,7 +1877,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B11" s="7">
         <v>43897</v>
       </c>
@@ -1869,7 +1888,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="7">
         <v>43897</v>
       </c>
@@ -1880,7 +1899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13" s="7">
         <v>43899</v>
       </c>
@@ -1891,7 +1910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B14" s="7">
         <v>43899</v>
       </c>
@@ -1902,13 +1921,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D15">
         <f>SUM(D3:D14)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>47</v>
       </c>
@@ -1923,16 +1942,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A059C0DF-3E9D-4D01-B549-9733ADE07856}">
   <dimension ref="B2:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -1943,7 +1962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" s="7">
         <v>43904</v>
       </c>
@@ -1954,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" s="7">
         <v>43904</v>
       </c>
@@ -1965,7 +1984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" s="7">
         <v>43911</v>
       </c>
@@ -1976,7 +1995,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="7">
         <v>43911</v>
       </c>
@@ -1987,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>43911</v>
       </c>
@@ -1998,7 +2017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B8" s="7">
         <v>43916</v>
       </c>
@@ -2009,7 +2028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B9" s="7">
         <v>43916</v>
       </c>
@@ -2020,7 +2039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B10" s="7">
         <v>43916</v>
       </c>
@@ -2031,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B11" s="7">
         <v>43916</v>
       </c>
@@ -2042,27 +2061,149 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D17">
         <f>SUM(D3:D11)</f>
         <v>13.5</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
         <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2421883F-D822-4CF1-AB76-9530ED988CE5}">
+  <dimension ref="B2:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="7">
+        <v>43923</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B4" s="7">
+        <v>43923</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="7">
+        <v>43926</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="7">
+        <v>43926</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="7">
+        <v>43926</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="7">
+        <v>43926</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D17">
+        <f>SUM(D3:D11)</f>
+        <v>9.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unicheck Test web + planif + test MySQL et FTP
Etat de l'art II, encore certains points à finaliser
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D292A975-7E53-4AFB-B7C7-4BB658F0A0F0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C612F-6EE7-4616-AA9F-F86C1B049E07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="4" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="SPRINT 0" sheetId="3" r:id="rId3"/>
     <sheet name="SPRINT 1" sheetId="4" r:id="rId4"/>
     <sheet name="SPRINT 2" sheetId="5" r:id="rId5"/>
+    <sheet name="SPRINT 3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -233,6 +234,48 @@
   </si>
   <si>
     <t>Unicheck Etat art</t>
+  </si>
+  <si>
+    <t>Planification, sprint review, Copyleaks test</t>
+  </si>
+  <si>
+    <t>Unicheck interface web</t>
+  </si>
+  <si>
+    <t>Unicheck test API</t>
+  </si>
+  <si>
+    <t>Unicheck appel support technique, email</t>
+  </si>
+  <si>
+    <t>Planification</t>
+  </si>
+  <si>
+    <t>Test connections FTP, HTTP</t>
+  </si>
+  <si>
+    <t>Test MYSQL connection</t>
+  </si>
+  <si>
+    <t>Dessiner schéma collaboratif du projet</t>
+  </si>
+  <si>
+    <t>Test page local XAMPP</t>
+  </si>
+  <si>
+    <t>Total projet</t>
+  </si>
+  <si>
+    <t>Temps avant rendu</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Temps total à réaliser</t>
+  </si>
+  <si>
+    <t>Cmb travailler par j</t>
   </si>
 </sst>
 </file>
@@ -292,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -307,6 +350,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +670,8 @@
   </sheetPr>
   <dimension ref="A3:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1663,114 +1707,156 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8302CA45-31B6-4463-AEAD-E85456601763}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1">
+        <f>'SPRINT 0'!A1+'SPRINT 1'!A1+'SPRINT 2'!A1+'SPRINT 3'!A1</f>
+        <v>47.25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B3" s="6">
         <v>43879</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C3" s="6">
         <v>43899</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B4" s="6">
         <v>43909</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C4" s="6">
         <v>43936</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B5" s="6">
         <v>43937</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C5" s="6">
         <v>43964</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B6" s="6">
         <v>43965</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C6" s="6">
         <v>43992</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B7" s="6">
         <v>43993</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C7" s="6">
         <v>44020</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B8" s="6">
         <v>44021</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C8" s="6">
         <v>44041</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="7">
+        <v>44043</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="8">
+        <f ca="1">C11-TODAY()</f>
+        <v>105</v>
+      </c>
+      <c r="D12">
+        <f ca="1">(F1-B1)/C12</f>
+        <v>2.6928571428571431</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C400973-BE12-4374-A59C-9A57E0EEF3E6}">
-  <dimension ref="B2:D17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1778,7 +1864,13 @@
     <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <f>SUM(D3:D14)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -1789,7 +1881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" s="7">
         <v>43879</v>
       </c>
@@ -1800,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="7">
         <v>43885</v>
       </c>
@@ -1811,7 +1903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="7">
         <v>43885</v>
       </c>
@@ -1822,7 +1914,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="7">
         <v>43885</v>
       </c>
@@ -1833,7 +1925,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>43885</v>
       </c>
@@ -1844,7 +1936,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="7">
         <v>43885</v>
       </c>
@@ -1855,7 +1947,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="7">
         <v>43889</v>
       </c>
@@ -1866,7 +1958,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="7">
         <v>43889</v>
       </c>
@@ -1877,7 +1969,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B11" s="7">
         <v>43897</v>
       </c>
@@ -1888,7 +1980,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B12" s="7">
         <v>43897</v>
       </c>
@@ -1899,7 +1991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B13" s="7">
         <v>43899</v>
       </c>
@@ -1910,7 +2002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B14" s="7">
         <v>43899</v>
       </c>
@@ -1921,7 +2013,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D15">
         <f>SUM(D3:D14)</f>
         <v>11</v>
@@ -1940,10 +2032,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A059C0DF-3E9D-4D01-B549-9733ADE07856}">
-  <dimension ref="B2:D18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1951,7 +2043,13 @@
     <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <f>SUM(D3:D11)</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -1962,7 +2060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" s="7">
         <v>43904</v>
       </c>
@@ -1973,7 +2071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="7">
         <v>43904</v>
       </c>
@@ -1984,7 +2082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="7">
         <v>43911</v>
       </c>
@@ -1995,7 +2093,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="7">
         <v>43911</v>
       </c>
@@ -2006,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>43911</v>
       </c>
@@ -2017,7 +2115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="7">
         <v>43916</v>
       </c>
@@ -2028,7 +2126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="7">
         <v>43916</v>
       </c>
@@ -2039,7 +2137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="7">
         <v>43916</v>
       </c>
@@ -2050,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B11" s="7">
         <v>43916</v>
       </c>
@@ -2061,16 +2159,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.45">
@@ -2091,10 +2189,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2421883F-D822-4CF1-AB76-9530ED988CE5}">
-  <dimension ref="B2:D17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2102,7 +2200,13 @@
     <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <f>SUM(D3:D11)</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2113,7 +2217,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" s="7">
         <v>43923</v>
       </c>
@@ -2124,7 +2228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="7">
         <v>43923</v>
       </c>
@@ -2135,7 +2239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="7">
         <v>43926</v>
       </c>
@@ -2146,7 +2250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="7">
         <v>43926</v>
       </c>
@@ -2157,7 +2261,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>43926</v>
       </c>
@@ -2168,7 +2272,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="7">
         <v>43926</v>
       </c>
@@ -2179,31 +2283,183 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="7">
+        <v>43930</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D17">
         <f>SUM(D3:D11)</f>
-        <v>9.5</v>
+        <v>14.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5E1D13-3593-4379-9475-09BDD7E3637B}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <f>SUM(D3:D11)</f>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="7">
+        <v>43932</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B4" s="7">
+        <v>43937</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="7">
+        <v>43937</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="7">
+        <v>43937</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="7">
+        <v>43937</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="7">
+        <v>43938</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="7">
+        <v>43938</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="7">
+        <v>43938</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D17">
+        <f>SUM(D3:D11)</f>
+        <v>8.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Draw schema-not done yet
Also tested Unicheck, now working!
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C612F-6EE7-4616-AA9F-F86C1B049E07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD070A4D-044D-460F-AC9C-391159EA8C2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="5" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>Cmb travailler par j</t>
+  </si>
+  <si>
+    <t>Test unicheck upload PDF - ça marche!</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8302CA45-31B6-4463-AEAD-E85456601763}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1726,7 +1729,7 @@
       </c>
       <c r="B1">
         <f>'SPRINT 0'!A1+'SPRINT 1'!A1+'SPRINT 2'!A1+'SPRINT 3'!A1</f>
-        <v>47.25</v>
+        <v>49.75</v>
       </c>
       <c r="E1" t="s">
         <v>77</v>
@@ -1842,7 +1845,7 @@
       </c>
       <c r="D12">
         <f ca="1">(F1-B1)/C12</f>
-        <v>2.6928571428571431</v>
+        <v>2.6690476190476189</v>
       </c>
     </row>
   </sheetData>
@@ -2327,8 +2330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5E1D13-3593-4379-9475-09BDD7E3637B}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2339,7 +2342,7 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1">
         <f>SUM(D3:D11)</f>
-        <v>8.25</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -2442,7 +2445,15 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B11" s="7"/>
+      <c r="B11" s="7">
+        <v>43938</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B12" s="7"/>
@@ -2459,7 +2470,7 @@
     <row r="17" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D17">
         <f>SUM(D3:D11)</f>
-        <v>8.25</v>
+        <v>10.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Etat de l'art II - comparaison
Finalisation et comparaison
Il faut encore mettre à jour le texte, mettre au propre
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD070A4D-044D-460F-AC9C-391159EA8C2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE598ADD-AF8C-4484-AA06-00BE5073FE90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="5" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>Test unicheck upload PDF - ça marche!</t>
+  </si>
+  <si>
+    <t>Test Copyleaks API</t>
+  </si>
+  <si>
+    <t>Test connection FTP server dev</t>
+  </si>
+  <si>
+    <t>Comparaison des outils, calcul prix</t>
   </si>
 </sst>
 </file>
@@ -1841,11 +1850,11 @@
       </c>
       <c r="C12" s="8">
         <f ca="1">C11-TODAY()</f>
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D12">
         <f ca="1">(F1-B1)/C12</f>
-        <v>2.6690476190476189</v>
+        <v>2.7747524752475248</v>
       </c>
     </row>
   </sheetData>
@@ -2331,7 +2340,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2456,21 +2465,53 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B12" s="7"/>
+      <c r="B12" s="7">
+        <v>43942</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B13" s="7"/>
+      <c r="B13" s="7">
+        <v>43942</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B14" s="7"/>
+      <c r="B14" s="7">
+        <v>43942</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B15" s="7"/>
+      <c r="B15" s="7">
+        <v>43942</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D17">
-        <f>SUM(D3:D11)</f>
-        <v>10.75</v>
+        <f>SUM(D3:D15)</f>
+        <v>13.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Etat art II - Tests 50 articles
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE598ADD-AF8C-4484-AA06-00BE5073FE90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACE5FE4-822D-4E7D-AD8E-946BD4C9755A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="5" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="6" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="SPRINT 1" sheetId="4" r:id="rId4"/>
     <sheet name="SPRINT 2" sheetId="5" r:id="rId5"/>
     <sheet name="SPRINT 3" sheetId="6" r:id="rId6"/>
+    <sheet name="SPRINT 4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -288,6 +289,36 @@
   </si>
   <si>
     <t>Comparaison des outils, calcul prix</t>
+  </si>
+  <si>
+    <t>Sprint 3 review + rencontre TB</t>
+  </si>
+  <si>
+    <t>Test DB</t>
+  </si>
+  <si>
+    <t>Manually create raw .txt files for articles</t>
+  </si>
+  <si>
+    <t>Meeting with Zhan : front-end demo</t>
+  </si>
+  <si>
+    <t>Raw text files - 50 articles</t>
+  </si>
+  <si>
+    <t>PHP script loop test</t>
+  </si>
+  <si>
+    <t>Copyleaks - Test</t>
+  </si>
+  <si>
+    <t>Unicheck - Tests 50</t>
+  </si>
+  <si>
+    <t>Prepostseo - Tests 50, manually</t>
+  </si>
+  <si>
+    <t>PlagiarismSearch - Tests 50 - script</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1753,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1737,8 +1768,8 @@
         <v>74</v>
       </c>
       <c r="B1">
-        <f>'SPRINT 0'!A1+'SPRINT 1'!A1+'SPRINT 2'!A1+'SPRINT 3'!A1</f>
-        <v>49.75</v>
+        <f>'SPRINT 0'!A1+'SPRINT 1'!A1+'SPRINT 2'!A1+'SPRINT 3'!A1+'SPRINT 4'!A1</f>
+        <v>66.25</v>
       </c>
       <c r="E1" t="s">
         <v>77</v>
@@ -1850,11 +1881,11 @@
       </c>
       <c r="C12" s="8">
         <f ca="1">C11-TODAY()</f>
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D12">
         <f ca="1">(F1-B1)/C12</f>
-        <v>2.7747524752475248</v>
+        <v>3.066860465116279</v>
       </c>
     </row>
   </sheetData>
@@ -1868,7 +1899,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2339,8 +2370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5E1D13-3593-4379-9475-09BDD7E3637B}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2508,10 +2539,184 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B16" s="7">
+        <v>43944</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D17">
-        <f>SUM(D3:D15)</f>
-        <v>13.75</v>
+        <f>SUM(D3:D16)</f>
+        <v>14.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2907829D-CE2F-4306-AC46-EF97BD5EEA67}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="32.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <f>SUM(D3:D11)</f>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="7">
+        <v>43951</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B4" s="7">
+        <v>43951</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="7">
+        <v>43951</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="7">
+        <v>43953</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="7">
+        <v>43953</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="7">
+        <v>43956</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="7">
+        <v>43956</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="7">
+        <v>43956</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B11" s="7">
+        <v>43957</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="7">
+        <v>43957</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D17">
+        <f>SUM(D3:D16)</f>
+        <v>21.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Etat art II - Mise en page et résultats des tests
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACE5FE4-822D-4E7D-AD8E-946BD4C9755A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B07821-0D7A-455D-985B-966BC0969C6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="6" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -319,6 +319,12 @@
   </si>
   <si>
     <t>PlagiarismSearch - Tests 50 - script</t>
+  </si>
+  <si>
+    <t>Mise en page etat art II</t>
+  </si>
+  <si>
+    <t>Discussion TB - Zhan + Nicole</t>
   </si>
 </sst>
 </file>
@@ -1881,11 +1887,11 @@
       </c>
       <c r="C12" s="8">
         <f ca="1">C11-TODAY()</f>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12">
         <f ca="1">(F1-B1)/C12</f>
-        <v>3.066860465116279</v>
+        <v>3.1029411764705883</v>
       </c>
     </row>
   </sheetData>
@@ -2566,7 +2572,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2702,10 +2708,26 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B13" s="7"/>
+      <c r="B13" s="7">
+        <v>43958</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B14" s="7"/>
+      <c r="B14" s="7">
+        <v>43958</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
@@ -2716,7 +2738,7 @@
     <row r="17" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D17">
         <f>SUM(D3:D16)</f>
-        <v>21.5</v>
+        <v>24.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SPRINT 4 - TEST RESULTS
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B07821-0D7A-455D-985B-966BC0969C6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ED15E2-06DE-45C4-B257-814444725B8B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="6" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
+    <workbookView xWindow="1905" yWindow="1425" windowWidth="20925" windowHeight="18090" activeTab="7" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="SPRINT 2" sheetId="5" r:id="rId5"/>
     <sheet name="SPRINT 3" sheetId="6" r:id="rId6"/>
     <sheet name="SPRINT 4" sheetId="7" r:id="rId7"/>
+    <sheet name="SPRINT 5" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -325,6 +326,18 @@
   </si>
   <si>
     <t>Discussion TB - Zhan + Nicole</t>
+  </si>
+  <si>
+    <t>Discussion Zhan</t>
+  </si>
+  <si>
+    <t>Etat art - Réseaux sociaux + paraphrasing</t>
+  </si>
+  <si>
+    <t>Compréhension code</t>
+  </si>
+  <si>
+    <t>AddArticle</t>
   </si>
 </sst>
 </file>
@@ -723,18 +736,18 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43878</v>
       </c>
@@ -757,7 +770,7 @@
         <v>43884</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -768,7 +781,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>G3+1</f>
         <v>43885</v>
@@ -798,7 +811,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -806,7 +819,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>G5+1</f>
         <v>43892</v>
@@ -836,7 +849,7 @@
         <v>43898</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -847,7 +860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>G7+1</f>
         <v>43899</v>
@@ -877,7 +890,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -888,7 +901,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>G9+1</f>
         <v>43906</v>
@@ -918,7 +931,7 @@
         <v>43912</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -927,7 +940,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>G11+1</f>
         <v>43913</v>
@@ -957,7 +970,7 @@
         <v>43919</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -970,7 +983,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f>G13+1</f>
         <v>43920</v>
@@ -1000,7 +1013,7 @@
         <v>43926</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1009,7 +1022,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f>G15+1</f>
         <v>43927</v>
@@ -1039,7 +1052,7 @@
         <v>43933</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
@@ -1052,7 +1065,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f>G17+1</f>
         <v>43934</v>
@@ -1082,7 +1095,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1091,7 +1104,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f>G19+1</f>
         <v>43941</v>
@@ -1121,7 +1134,7 @@
         <v>43947</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
@@ -1134,7 +1147,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f>G21+1</f>
         <v>43948</v>
@@ -1164,7 +1177,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1173,7 +1186,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f>G23+1</f>
         <v>43955</v>
@@ -1203,7 +1216,7 @@
         <v>43961</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
@@ -1216,7 +1229,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f>G25+1</f>
         <v>43962</v>
@@ -1246,7 +1259,7 @@
         <v>43968</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1255,7 +1268,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f>G27+1</f>
         <v>43969</v>
@@ -1285,7 +1298,7 @@
         <v>43975</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
@@ -1298,7 +1311,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f>G29+1</f>
         <v>43976</v>
@@ -1328,7 +1341,7 @@
         <v>43982</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1337,7 +1350,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f>G31+1</f>
         <v>43983</v>
@@ -1367,7 +1380,7 @@
         <v>43989</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
@@ -1380,7 +1393,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f>G33+1</f>
         <v>43990</v>
@@ -1410,7 +1423,7 @@
         <v>43996</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1419,7 +1432,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f>G35+1</f>
         <v>43997</v>
@@ -1449,7 +1462,7 @@
         <v>44003</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -1462,7 +1475,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f>G37+1</f>
         <v>44004</v>
@@ -1492,7 +1505,7 @@
         <v>44010</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1501,7 +1514,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f>G39+1</f>
         <v>44011</v>
@@ -1531,7 +1544,7 @@
         <v>44017</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
@@ -1544,7 +1557,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f>G41+1</f>
         <v>44018</v>
@@ -1574,7 +1587,7 @@
         <v>44024</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1583,7 +1596,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f>G43+1</f>
         <v>44025</v>
@@ -1613,7 +1626,7 @@
         <v>44031</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
@@ -1626,7 +1639,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <f>G45+1</f>
         <v>44032</v>
@@ -1656,7 +1669,7 @@
         <v>44038</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1665,7 +1678,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f>G47+1</f>
         <v>44039</v>
@@ -1695,7 +1708,7 @@
         <v>44045</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="5" t="s">
@@ -1708,7 +1721,7 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f>G49+1</f>
         <v>44046</v>
@@ -1738,7 +1751,7 @@
         <v>44052</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1762,20 +1775,20 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
       <c r="B1">
         <f>'SPRINT 0'!A1+'SPRINT 1'!A1+'SPRINT 2'!A1+'SPRINT 3'!A1+'SPRINT 4'!A1</f>
-        <v>66.25</v>
+        <v>74.25</v>
       </c>
       <c r="E1" t="s">
         <v>77</v>
@@ -1784,7 +1797,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -1796,7 +1809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1810,7 +1823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1822,7 +1835,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1834,7 +1847,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1846,7 +1859,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1858,7 +1871,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1870,7 +1883,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>76</v>
       </c>
@@ -1881,17 +1894,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
       <c r="C12" s="8">
         <f ca="1">C11-TODAY()</f>
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D12">
         <f ca="1">(F1-B1)/C12</f>
-        <v>3.1029411764705883</v>
+        <v>3.875</v>
       </c>
     </row>
   </sheetData>
@@ -1908,18 +1921,18 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D14)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -1930,7 +1943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43879</v>
       </c>
@@ -1941,7 +1954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43885</v>
       </c>
@@ -1952,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43885</v>
       </c>
@@ -1963,7 +1976,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43885</v>
       </c>
@@ -1974,7 +1987,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43885</v>
       </c>
@@ -1985,7 +1998,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43885</v>
       </c>
@@ -1996,7 +2009,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43889</v>
       </c>
@@ -2007,7 +2020,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>43889</v>
       </c>
@@ -2018,7 +2031,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>43897</v>
       </c>
@@ -2029,7 +2042,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>43897</v>
       </c>
@@ -2040,7 +2053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>43899</v>
       </c>
@@ -2051,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>43899</v>
       </c>
@@ -2062,13 +2075,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15">
         <f>SUM(D3:D14)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>47</v>
       </c>
@@ -2087,18 +2100,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D11)</f>
         <v>13.5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2109,7 +2122,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43904</v>
       </c>
@@ -2120,7 +2133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43904</v>
       </c>
@@ -2131,7 +2144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43911</v>
       </c>
@@ -2142,7 +2155,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43911</v>
       </c>
@@ -2153,7 +2166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43911</v>
       </c>
@@ -2164,7 +2177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43916</v>
       </c>
@@ -2175,7 +2188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43916</v>
       </c>
@@ -2186,7 +2199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>43916</v>
       </c>
@@ -2197,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>43916</v>
       </c>
@@ -2208,25 +2221,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D11)</f>
         <v>13.5</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>55</v>
       </c>
@@ -2244,18 +2257,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D11)</f>
         <v>14.5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2266,7 +2279,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43923</v>
       </c>
@@ -2277,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43923</v>
       </c>
@@ -2288,7 +2301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43926</v>
       </c>
@@ -2299,7 +2312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43926</v>
       </c>
@@ -2310,7 +2323,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43926</v>
       </c>
@@ -2321,7 +2334,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43926</v>
       </c>
@@ -2332,7 +2345,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43930</v>
       </c>
@@ -2343,25 +2356,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D11)</f>
         <v>14.5</v>
@@ -2380,18 +2393,18 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D11)</f>
         <v>10.75</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2402,7 +2415,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43932</v>
       </c>
@@ -2413,7 +2426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43937</v>
       </c>
@@ -2424,7 +2437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43937</v>
       </c>
@@ -2435,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43937</v>
       </c>
@@ -2446,7 +2459,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43937</v>
       </c>
@@ -2457,7 +2470,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43938</v>
       </c>
@@ -2468,7 +2481,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43938</v>
       </c>
@@ -2479,7 +2492,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>43938</v>
       </c>
@@ -2490,7 +2503,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>43938</v>
       </c>
@@ -2501,7 +2514,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>43942</v>
       </c>
@@ -2512,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>43942</v>
       </c>
@@ -2523,7 +2536,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>43942</v>
       </c>
@@ -2534,7 +2547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>43942</v>
       </c>
@@ -2545,7 +2558,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>43944</v>
       </c>
@@ -2556,7 +2569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D16)</f>
         <v>14.75</v>
@@ -2571,22 +2584,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2907829D-CE2F-4306-AC46-EF97BD5EEA67}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
-        <f>SUM(D3:D11)</f>
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <f>SUM(D3:D14)</f>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2597,7 +2610,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43951</v>
       </c>
@@ -2608,7 +2621,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43951</v>
       </c>
@@ -2619,7 +2632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43951</v>
       </c>
@@ -2630,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43953</v>
       </c>
@@ -2641,7 +2654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43953</v>
       </c>
@@ -2652,7 +2665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43956</v>
       </c>
@@ -2663,7 +2676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43956</v>
       </c>
@@ -2674,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>43956</v>
       </c>
@@ -2685,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>43957</v>
       </c>
@@ -2696,7 +2709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>43957</v>
       </c>
@@ -2707,7 +2720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>43958</v>
       </c>
@@ -2718,7 +2731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>43958</v>
       </c>
@@ -2729,16 +2742,136 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D16)</f>
         <v>24.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F06ED0-EB85-45D1-9FA2-E9044C3B1584}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>SUM(D3:D14)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="7">
+        <v>43964</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <v>43968</v>
+      </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>43977</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>43977</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>43977</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>SUM(D3:D16)</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create report with api
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\HES\TB\OJILTRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11B0B34-4F5E-47D5-AB06-2F821149449B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6F7C87-CE3E-4FE8-81F5-1ED53062D3F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="38700" windowHeight="15195" firstSheet="1" activeTab="9" xr2:uid="{77428253-80D6-43E1-BA38-7FEDA69236BC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="SPRINT 4" sheetId="7" r:id="rId7"/>
     <sheet name="SPRINT 5" sheetId="8" r:id="rId8"/>
     <sheet name="SPRINT 6" sheetId="9" r:id="rId9"/>
+    <sheet name="SPRINT 7" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="109">
   <si>
     <t>FIN SPRINT 1</t>
   </si>
@@ -360,6 +361,15 @@
   </si>
   <si>
     <t>Planning update</t>
+  </si>
+  <si>
+    <t>Sprint review + comments</t>
+  </si>
+  <si>
+    <t>Créer rapport avec API</t>
+  </si>
+  <si>
+    <t>Planification, git</t>
   </si>
 </sst>
 </file>
@@ -758,18 +768,18 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43878</v>
       </c>
@@ -792,7 +802,7 @@
         <v>43884</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -803,7 +813,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>G3+1</f>
         <v>43885</v>
@@ -833,7 +843,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -841,7 +851,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>G5+1</f>
         <v>43892</v>
@@ -871,7 +881,7 @@
         <v>43898</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -882,7 +892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>G7+1</f>
         <v>43899</v>
@@ -912,7 +922,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -923,7 +933,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>G9+1</f>
         <v>43906</v>
@@ -953,7 +963,7 @@
         <v>43912</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -962,7 +972,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>G11+1</f>
         <v>43913</v>
@@ -992,7 +1002,7 @@
         <v>43919</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -1005,7 +1015,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f>G13+1</f>
         <v>43920</v>
@@ -1035,7 +1045,7 @@
         <v>43926</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1044,7 +1054,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f>G15+1</f>
         <v>43927</v>
@@ -1074,7 +1084,7 @@
         <v>43933</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
@@ -1087,7 +1097,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f>G17+1</f>
         <v>43934</v>
@@ -1117,7 +1127,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1126,7 +1136,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f>G19+1</f>
         <v>43941</v>
@@ -1156,7 +1166,7 @@
         <v>43947</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
@@ -1169,7 +1179,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f>G21+1</f>
         <v>43948</v>
@@ -1199,7 +1209,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1208,7 +1218,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f>G23+1</f>
         <v>43955</v>
@@ -1238,7 +1248,7 @@
         <v>43961</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
@@ -1251,7 +1261,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f>G25+1</f>
         <v>43962</v>
@@ -1281,7 +1291,7 @@
         <v>43968</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1290,7 +1300,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f>G27+1</f>
         <v>43969</v>
@@ -1320,7 +1330,7 @@
         <v>43975</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
@@ -1333,7 +1343,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f>G29+1</f>
         <v>43976</v>
@@ -1363,7 +1373,7 @@
         <v>43982</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1372,7 +1382,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f>G31+1</f>
         <v>43983</v>
@@ -1402,7 +1412,7 @@
         <v>43989</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
@@ -1415,7 +1425,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f>G33+1</f>
         <v>43990</v>
@@ -1445,7 +1455,7 @@
         <v>43996</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1454,7 +1464,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f>G35+1</f>
         <v>43997</v>
@@ -1484,7 +1494,7 @@
         <v>44003</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -1497,7 +1507,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f>G37+1</f>
         <v>44004</v>
@@ -1527,7 +1537,7 @@
         <v>44010</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1536,7 +1546,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f>G39+1</f>
         <v>44011</v>
@@ -1566,7 +1576,7 @@
         <v>44017</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
@@ -1579,7 +1589,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f>G41+1</f>
         <v>44018</v>
@@ -1609,7 +1619,7 @@
         <v>44024</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1618,7 +1628,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f>G43+1</f>
         <v>44025</v>
@@ -1648,7 +1658,7 @@
         <v>44031</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
@@ -1661,7 +1671,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <f>G45+1</f>
         <v>44032</v>
@@ -1691,7 +1701,7 @@
         <v>44038</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1700,7 +1710,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f>G47+1</f>
         <v>44039</v>
@@ -1730,7 +1740,7 @@
         <v>44045</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="5" t="s">
@@ -1743,7 +1753,7 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f>G49+1</f>
         <v>44046</v>
@@ -1773,7 +1783,7 @@
         <v>44052</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1789,22 +1799,142 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB3F2D1-547E-46DA-B3FF-B3925AE2305A}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>SUM(D3:D14)</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="7">
+        <v>44015</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <v>44015</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>44021</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>44025</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>44025</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>SUM(D3:D16)</f>
+        <v>14.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8302CA45-31B6-4463-AEAD-E85456601763}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -1819,7 +1949,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -1831,7 +1961,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1845,7 +1975,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1857,7 +1987,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1869,7 +1999,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1881,7 +2011,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1893,7 +2023,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1905,7 +2035,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>76</v>
       </c>
@@ -1916,17 +2046,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
       <c r="C12" s="8">
         <f ca="1">C11-TODAY()</f>
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <f ca="1">(F1-B1)/C12</f>
-        <v>6.0892857142857144</v>
+        <v>14.208333333333334</v>
       </c>
     </row>
   </sheetData>
@@ -1940,21 +2070,21 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D14)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -1965,7 +2095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43879</v>
       </c>
@@ -1976,7 +2106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43885</v>
       </c>
@@ -1987,7 +2117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43885</v>
       </c>
@@ -1998,7 +2128,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43885</v>
       </c>
@@ -2009,7 +2139,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43885</v>
       </c>
@@ -2020,7 +2150,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43885</v>
       </c>
@@ -2031,7 +2161,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43889</v>
       </c>
@@ -2042,7 +2172,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>43889</v>
       </c>
@@ -2053,7 +2183,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>43897</v>
       </c>
@@ -2064,7 +2194,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>43897</v>
       </c>
@@ -2075,7 +2205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>43899</v>
       </c>
@@ -2086,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>43899</v>
       </c>
@@ -2097,13 +2227,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15">
         <f>SUM(D3:D14)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>47</v>
       </c>
@@ -2122,18 +2252,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D11)</f>
         <v>13.5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2144,7 +2274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43904</v>
       </c>
@@ -2155,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43904</v>
       </c>
@@ -2166,7 +2296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43911</v>
       </c>
@@ -2177,7 +2307,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43911</v>
       </c>
@@ -2188,7 +2318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43911</v>
       </c>
@@ -2199,7 +2329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43916</v>
       </c>
@@ -2210,7 +2340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43916</v>
       </c>
@@ -2221,7 +2351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>43916</v>
       </c>
@@ -2232,7 +2362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>43916</v>
       </c>
@@ -2243,25 +2373,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D11)</f>
         <v>13.5</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>55</v>
       </c>
@@ -2279,18 +2409,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D11)</f>
         <v>14.5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2301,7 +2431,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43923</v>
       </c>
@@ -2312,7 +2442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43923</v>
       </c>
@@ -2323,7 +2453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43926</v>
       </c>
@@ -2334,7 +2464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43926</v>
       </c>
@@ -2345,7 +2475,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43926</v>
       </c>
@@ -2356,7 +2486,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43926</v>
       </c>
@@ -2367,7 +2497,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43930</v>
       </c>
@@ -2378,25 +2508,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D11)</f>
         <v>14.5</v>
@@ -2415,18 +2545,18 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D11)</f>
         <v>10.75</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2437,7 +2567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43932</v>
       </c>
@@ -2448,7 +2578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43937</v>
       </c>
@@ -2459,7 +2589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43937</v>
       </c>
@@ -2470,7 +2600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43937</v>
       </c>
@@ -2481,7 +2611,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43937</v>
       </c>
@@ -2492,7 +2622,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43938</v>
       </c>
@@ -2503,7 +2633,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43938</v>
       </c>
@@ -2514,7 +2644,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>43938</v>
       </c>
@@ -2525,7 +2655,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>43938</v>
       </c>
@@ -2536,7 +2666,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>43942</v>
       </c>
@@ -2547,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>43942</v>
       </c>
@@ -2558,7 +2688,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>43942</v>
       </c>
@@ -2569,7 +2699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>43942</v>
       </c>
@@ -2580,7 +2710,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>43944</v>
       </c>
@@ -2591,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D16)</f>
         <v>14.75</v>
@@ -2610,18 +2740,18 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D14)</f>
         <v>24.5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2632,7 +2762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43951</v>
       </c>
@@ -2643,7 +2773,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43951</v>
       </c>
@@ -2654,7 +2784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43951</v>
       </c>
@@ -2665,7 +2795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43953</v>
       </c>
@@ -2676,7 +2806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43953</v>
       </c>
@@ -2687,7 +2817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>43956</v>
       </c>
@@ -2698,7 +2828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>43956</v>
       </c>
@@ -2709,7 +2839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>43956</v>
       </c>
@@ -2720,7 +2850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>43957</v>
       </c>
@@ -2731,7 +2861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>43957</v>
       </c>
@@ -2742,7 +2872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>43958</v>
       </c>
@@ -2753,7 +2883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>43958</v>
       </c>
@@ -2764,13 +2894,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D16)</f>
         <v>24.5</v>
@@ -2786,21 +2916,21 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.9296875" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D14)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2811,7 +2941,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43964</v>
       </c>
@@ -2822,7 +2952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43968</v>
       </c>
@@ -2833,7 +2963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43977</v>
       </c>
@@ -2844,7 +2974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43977</v>
       </c>
@@ -2855,7 +2985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43977</v>
       </c>
@@ -2866,34 +2996,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D16)</f>
         <v>10</v>
@@ -2909,21 +3039,21 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.9296875" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(D3:D14)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -2934,7 +3064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>43990</v>
       </c>
@@ -2945,7 +3075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>43991</v>
       </c>
@@ -2956,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>43991</v>
       </c>
@@ -2967,7 +3097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>43992</v>
       </c>
@@ -2978,7 +3108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>43994</v>
       </c>
@@ -2989,7 +3119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>44000</v>
       </c>
@@ -3000,7 +3130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>44001</v>
       </c>
@@ -3011,28 +3141,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D16)</f>
         <v>14</v>

</xml_diff>